<commit_message>
finish report from lab_4
</commit_message>
<xml_diff>
--- a/Our_Labs/Lab_4/Lab_4.xlsx
+++ b/Our_Labs/Lab_4/Lab_4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\OneDrive\Pulpit\Szkoła\fizyka\moje_sprawka\repo\Fizyka\Our_Labs\Lab_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piter\Desktop\Git_repos\Fizyka\Our_Labs\Lab_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C134FFE8-9624-4547-AF7A-7D1D22BB6602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89262DA-2CB3-45B3-8EC5-25C85A334F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6ABC6EA7-95B5-4EB7-8382-A789AC46FAE8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ABC6EA7-95B5-4EB7-8382-A789AC46FAE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -233,72 +233,17 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Zależność okresu drgań od pojemności T(C)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10681285431165193"/>
-          <c:y val="0.17171296296296296"/>
-          <c:w val="0.74943142544984298"/>
-          <c:h val="0.72088764946048411"/>
+          <c:x val="0.13554132830532567"/>
+          <c:y val="2.8194444444444459E-2"/>
+          <c:w val="0.82607916214122346"/>
+          <c:h val="0.84763382236784912"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -815,72 +760,17 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Zależność okresu drgań od rezystancji T(R)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.4692038495188105E-2"/>
-          <c:y val="0.16708333333333336"/>
-          <c:w val="0.72590290344141761"/>
-          <c:h val="0.72088764946048411"/>
+          <c:x val="0.12880987436439872"/>
+          <c:y val="3.8633199070252359E-2"/>
+          <c:w val="0.82321139205425409"/>
+          <c:h val="0.85534155504578913"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1376,72 +1266,17 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Zależność okresu drgań od pojemności T(C)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10681285431165193"/>
-          <c:y val="0.17171296296296296"/>
-          <c:w val="0.74943142544984298"/>
-          <c:h val="0.72088764946048411"/>
+          <c:x val="0.14602856260614483"/>
+          <c:y val="4.3987546883271965E-2"/>
+          <c:w val="0.8198537903350317"/>
+          <c:h val="0.81534706645397281"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1962,64 +1797,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Zależność okresu drgań T od napięcia zasilania U</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15180309482824003"/>
+          <c:y val="4.4627241145230201E-2"/>
+          <c:w val="0.81506221755421393"/>
+          <c:h val="0.80654000494606293"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -4558,16 +4348,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>107372</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>3464</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>214248</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>119247</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>526472</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>45028</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>605642</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>183078</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4595,15 +4385,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>135084</xdr:colOff>
+      <xdr:colOff>135083</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>173184</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>173183</xdr:rowOff>
+      <xdr:colOff>367146</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13854</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4630,16 +4420,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>13854</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>249382</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>55418</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>20782</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4669,15 +4459,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>803564</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>10391</xdr:rowOff>
+      <xdr:colOff>125896</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109782</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>290946</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>51955</xdr:rowOff>
+      <xdr:colOff>265044</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4702,6 +4492,122 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>99392</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>125896</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="510209" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="pole tekstowe 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86B465D7-FD28-0082-18E5-51E519445CC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2663688" y="5691809"/>
+          <a:ext cx="510209" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>T, ms</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>424071</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>145775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="510209" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="pole tekstowe 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4780F2B7-C8CB-4A97-849D-3F2D118A3BC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7460975" y="8865705"/>
+          <a:ext cx="510209" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>U, V</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4709,12 +4615,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.01113</cdr:x>
-      <cdr:y>0.03662</cdr:y>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.10446</cdr:x>
-      <cdr:y>0.11742</cdr:y>
+      <cdr:x>0.09333</cdr:x>
+      <cdr:y>0.0808</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4729,8 +4635,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="63102" y="100445"/>
-          <a:ext cx="529180" cy="221674"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="551161" cy="266708"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4742,7 +4648,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>T(ms)</a:t>
+            <a:t>T,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>ms</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4750,12 +4664,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.87845</cdr:x>
-      <cdr:y>0.88763</cdr:y>
+      <cdr:x>0.92499</cdr:x>
+      <cdr:y>0.93525</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96993</cdr:x>
-      <cdr:y>0.97096</cdr:y>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4770,8 +4684,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5358053" y="2434936"/>
-          <a:ext cx="558028" cy="228600"/>
+          <a:off x="6000791" y="3592439"/>
+          <a:ext cx="486603" cy="248735"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4783,7 +4697,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>C(nF)</a:t>
+            <a:t>C,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>nF</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4834,12 +4756,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0065</cdr:x>
-      <cdr:y>0.03856</cdr:y>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.09422</cdr:x>
-      <cdr:y>0.14139</cdr:y>
+      <cdr:x>0.08772</cdr:x>
+      <cdr:y>0.10283</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4854,8 +4776,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="34636" y="103909"/>
-          <a:ext cx="467591" cy="277091"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="555098" cy="371837"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4867,7 +4789,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>T(ms)</a:t>
+            <a:t>T,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>ms</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -4878,11 +4808,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.85997</cdr:x>
-      <cdr:y>0.88432</cdr:y>
+      <cdr:x>0.91531</cdr:x>
+      <cdr:y>0.94179</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.94466</cdr:x>
+      <cdr:x>1</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -4898,8 +4828,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5275117" y="2382982"/>
-          <a:ext cx="519546" cy="311727"/>
+          <a:off x="5792139" y="3405550"/>
+          <a:ext cx="535924" cy="210485"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4911,7 +4841,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>R(k</a:t>
+            <a:t>R,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>k</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="el-GR" sz="1100">
@@ -4920,10 +4858,7 @@
             </a:rPr>
             <a:t>Ω</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>)</a:t>
-          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -4935,12 +4870,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.01113</cdr:x>
-      <cdr:y>0.03662</cdr:y>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.10446</cdr:x>
-      <cdr:y>0.11742</cdr:y>
+      <cdr:x>0.07558</cdr:x>
+      <cdr:y>0.0771</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4955,8 +4890,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="63102" y="100445"/>
-          <a:ext cx="529180" cy="221674"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="489550" cy="264901"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4968,7 +4903,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>T(ms)</a:t>
+            <a:t>T,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>ms</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4976,12 +4919,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.87845</cdr:x>
-      <cdr:y>0.88763</cdr:y>
+      <cdr:x>0.90852</cdr:x>
+      <cdr:y>0.91667</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96993</cdr:x>
-      <cdr:y>0.97096</cdr:y>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4996,8 +4939,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5358053" y="2434936"/>
-          <a:ext cx="558028" cy="228600"/>
+          <a:off x="5884484" y="3149611"/>
+          <a:ext cx="592516" cy="286316"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5009,7 +4952,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>C(nF)</a:t>
+            <a:t>C,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>nF</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -5317,8 +5268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA9AE06-1845-460E-B383-1A040F57105F}">
   <dimension ref="A2:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>